<commit_message>
tdf#166724 unit test: use Carlito, not Calibri as font
HOWEVER (even with this font change):
Stephan reports that his windows build still fails with
Test name: testTdf166724_cellAnchor::TestBody
equality assertion failed
- Expected: 1990
- Actual  : 1905

So, just remove the bits about specific width and height.
Those are very dependent on how the computer handles
"automatic row height", which could be affected by
lots of variables I imagine
(although it has passed lots of builds and backports).

make CppunitTest_sc_subsequent_export_test2 \
    CPPUNIT_TEST_NAME=testTdf166724_cellAnchor

Change-Id: I57e9b252ea82b0a065142653f6d68fb4ba44fe3b
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/195467
Tested-by: Jenkins
Reviewed-by: Justin Luth <jluth@mail.com>
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/tdf166724_cellAnchor.xlsx
+++ b/sc/qa/unit/data/xlsx/tdf166724_cellAnchor.xlsx
@@ -19,7 +19,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Carlito"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -138,7 +138,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Carlito"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>

</xml_diff>